<commit_message>
Rerunning, fixed 6PPDQ reaction rate
Rerunning, fixed 6PPDQ reaction rate from 8100 to 1800 hrs.
</commit_message>
<xml_diff>
--- a/inputfiles/6PPDQ_CHEMSUMM.xlsx
+++ b/inputfiles/6PPDQ_CHEMSUMM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\SubsurfaceSinks\inputfiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B0CE59-AC22-4C35-81EA-7AAE16938D1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFEBC782-6A7E-4CD1-BDB6-C3F51693978A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1088,7 +1088,7 @@
   <dimension ref="A1:U23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1195,7 @@
         <v>33</v>
       </c>
       <c r="G2" s="1">
-        <v>8100</v>
+        <v>1800</v>
       </c>
       <c r="H2" s="1">
         <f>0.1*900</f>

</xml_diff>